<commit_message>
adding files to repo
</commit_message>
<xml_diff>
--- a/Doc/Payroll-Claims-Form.xlsx
+++ b/Doc/Payroll-Claims-Form.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ven-talent-axwar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ven-talent-axwar\Documents\ACWAR\iApply_Integration\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF140586-1E6B-4334-AAD5-081B82A126F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07D9B5D-E780-41C8-AF61-446D91824640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1603,6 +1603,283 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1625,9 +1902,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1642,280 +1916,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2397,7 +2397,7 @@
   <dimension ref="B1:AC69"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE19" sqref="AE19"/>
+      <selection activeCell="B11" sqref="B11:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2444,43 +2444,43 @@
       <c r="O3" s="16"/>
       <c r="P3" s="16"/>
       <c r="Q3" s="16"/>
-      <c r="R3" s="84"/>
-      <c r="S3" s="84"/>
-      <c r="T3" s="84"/>
-      <c r="U3" s="84"/>
-      <c r="V3" s="84"/>
+      <c r="R3" s="168"/>
+      <c r="S3" s="168"/>
+      <c r="T3" s="168"/>
+      <c r="U3" s="168"/>
+      <c r="V3" s="168"/>
       <c r="W3" s="67"/>
     </row>
     <row r="4" spans="2:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="88" t="s">
+      <c r="C4" s="135" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="89"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="91"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="137"/>
+      <c r="G4" s="137"/>
+      <c r="H4" s="137"/>
+      <c r="I4" s="137"/>
+      <c r="J4" s="137"/>
+      <c r="K4" s="138"/>
       <c r="M4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="88" t="s">
+      <c r="N4" s="135" t="s">
         <v>146</v>
       </c>
-      <c r="O4" s="92"/>
+      <c r="O4" s="139"/>
       <c r="Q4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="R4" s="84"/>
-      <c r="S4" s="84"/>
-      <c r="T4" s="84"/>
-      <c r="U4" s="84"/>
-      <c r="V4" s="84"/>
+      <c r="R4" s="168"/>
+      <c r="S4" s="168"/>
+      <c r="T4" s="168"/>
+      <c r="U4" s="168"/>
+      <c r="V4" s="168"/>
       <c r="W4" s="67"/>
     </row>
     <row r="5" spans="2:29" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2492,35 +2492,35 @@
       <c r="B6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="93" t="s">
+      <c r="C6" s="140" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="94"/>
-      <c r="E6" s="94"/>
-      <c r="F6" s="94"/>
-      <c r="G6" s="94"/>
-      <c r="H6" s="94"/>
-      <c r="I6" s="94"/>
-      <c r="J6" s="94"/>
-      <c r="K6" s="95"/>
+      <c r="D6" s="141"/>
+      <c r="E6" s="141"/>
+      <c r="F6" s="141"/>
+      <c r="G6" s="141"/>
+      <c r="H6" s="141"/>
+      <c r="I6" s="141"/>
+      <c r="J6" s="141"/>
+      <c r="K6" s="142"/>
       <c r="M6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="88" t="s">
+      <c r="N6" s="135" t="s">
         <v>147</v>
       </c>
-      <c r="O6" s="92"/>
+      <c r="O6" s="139"/>
       <c r="P6" s="17"/>
       <c r="Q6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="R6" s="85">
-        <v>44703</v>
-      </c>
-      <c r="S6" s="85"/>
-      <c r="T6" s="85"/>
-      <c r="U6" s="85"/>
-      <c r="V6" s="85"/>
+      <c r="R6" s="169">
+        <v>44718</v>
+      </c>
+      <c r="S6" s="169"/>
+      <c r="T6" s="169"/>
+      <c r="U6" s="169"/>
+      <c r="V6" s="169"/>
       <c r="W6" s="68"/>
       <c r="AA6" s="19" t="s">
         <v>8</v>
@@ -2547,13 +2547,13 @@
       <c r="B8" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="96" t="s">
+      <c r="C8" s="143" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="81" t="s">
+      <c r="D8" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="81" t="s">
+      <c r="E8" s="76" t="s">
         <v>16</v>
       </c>
       <c r="F8" s="38" t="s">
@@ -2568,25 +2568,25 @@
       <c r="I8" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="99" t="s">
+      <c r="J8" s="146" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="100"/>
-      <c r="L8" s="100"/>
-      <c r="M8" s="100"/>
-      <c r="N8" s="101"/>
-      <c r="O8" s="102" t="s">
+      <c r="K8" s="147"/>
+      <c r="L8" s="147"/>
+      <c r="M8" s="147"/>
+      <c r="N8" s="148"/>
+      <c r="O8" s="149" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="103"/>
-      <c r="Q8" s="104"/>
-      <c r="R8" s="73" t="s">
+      <c r="P8" s="150"/>
+      <c r="Q8" s="151"/>
+      <c r="R8" s="158" t="s">
         <v>23</v>
       </c>
-      <c r="S8" s="74"/>
-      <c r="T8" s="74"/>
-      <c r="U8" s="74"/>
-      <c r="V8" s="75"/>
+      <c r="S8" s="159"/>
+      <c r="T8" s="159"/>
+      <c r="U8" s="159"/>
+      <c r="V8" s="160"/>
       <c r="AB8" t="s">
         <v>24</v>
       </c>
@@ -2598,9 +2598,9 @@
       <c r="B9" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="97"/>
-      <c r="D9" s="165"/>
-      <c r="E9" s="82"/>
+      <c r="C9" s="144"/>
+      <c r="D9" s="77"/>
+      <c r="E9" s="166"/>
       <c r="F9" s="41" t="s">
         <v>27</v>
       </c>
@@ -2625,17 +2625,17 @@
       <c r="M9" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="N9" s="79" t="s">
+      <c r="N9" s="164" t="s">
         <v>34</v>
       </c>
-      <c r="O9" s="105"/>
-      <c r="P9" s="106"/>
-      <c r="Q9" s="107"/>
-      <c r="R9" s="76"/>
-      <c r="S9" s="77"/>
-      <c r="T9" s="77"/>
-      <c r="U9" s="77"/>
-      <c r="V9" s="78"/>
+      <c r="O9" s="152"/>
+      <c r="P9" s="153"/>
+      <c r="Q9" s="154"/>
+      <c r="R9" s="161"/>
+      <c r="S9" s="162"/>
+      <c r="T9" s="162"/>
+      <c r="U9" s="162"/>
+      <c r="V9" s="163"/>
       <c r="AB9" t="s">
         <v>35</v>
       </c>
@@ -2647,9 +2647,9 @@
       <c r="B10" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="98"/>
-      <c r="D10" s="166"/>
-      <c r="E10" s="83"/>
+      <c r="C10" s="145"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="167"/>
       <c r="F10" s="47" t="s">
         <v>38</v>
       </c>
@@ -2674,10 +2674,10 @@
       <c r="M10" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="N10" s="80"/>
-      <c r="O10" s="108"/>
-      <c r="P10" s="109"/>
-      <c r="Q10" s="110"/>
+      <c r="N10" s="165"/>
+      <c r="O10" s="155"/>
+      <c r="P10" s="156"/>
+      <c r="Q10" s="157"/>
       <c r="R10" s="60"/>
       <c r="S10" s="61"/>
       <c r="T10" s="62"/>
@@ -2692,7 +2692,7 @@
     </row>
     <row r="11" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="37">
-        <v>44697</v>
+        <v>44711</v>
       </c>
       <c r="C11" s="20" t="str">
         <f t="shared" ref="C11:C18" si="0">IF(B11&lt;&gt;"",TEXT(B11,"DDD"),"")</f>
@@ -2714,9 +2714,9 @@
         <v>0</v>
       </c>
       <c r="N11" s="12"/>
-      <c r="O11" s="86"/>
-      <c r="P11" s="87"/>
-      <c r="Q11" s="87"/>
+      <c r="O11" s="132"/>
+      <c r="P11" s="133"/>
+      <c r="Q11" s="133"/>
       <c r="R11" s="52"/>
       <c r="S11" s="53"/>
       <c r="T11" s="53"/>
@@ -2731,7 +2731,7 @@
     </row>
     <row r="12" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="37">
-        <v>44698</v>
+        <v>44712</v>
       </c>
       <c r="C12" s="20" t="str">
         <f t="shared" si="0"/>
@@ -2753,9 +2753,9 @@
         <v>0</v>
       </c>
       <c r="N12" s="12"/>
-      <c r="O12" s="86"/>
-      <c r="P12" s="87"/>
-      <c r="Q12" s="87"/>
+      <c r="O12" s="132"/>
+      <c r="P12" s="133"/>
+      <c r="Q12" s="133"/>
       <c r="R12" s="52"/>
       <c r="S12" s="53"/>
       <c r="T12" s="53"/>
@@ -2767,7 +2767,7 @@
     </row>
     <row r="13" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="37">
-        <v>44699</v>
+        <v>44713</v>
       </c>
       <c r="C13" s="20" t="str">
         <f t="shared" si="0"/>
@@ -2789,9 +2789,9 @@
         <v>0</v>
       </c>
       <c r="N13" s="12"/>
-      <c r="O13" s="111"/>
-      <c r="P13" s="112"/>
-      <c r="Q13" s="112"/>
+      <c r="O13" s="130"/>
+      <c r="P13" s="131"/>
+      <c r="Q13" s="131"/>
       <c r="R13" s="55"/>
       <c r="S13" s="53"/>
       <c r="T13" s="56"/>
@@ -2803,7 +2803,7 @@
     </row>
     <row r="14" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="37">
-        <v>44700</v>
+        <v>44714</v>
       </c>
       <c r="C14" s="20" t="str">
         <f t="shared" si="0"/>
@@ -2825,9 +2825,9 @@
         <v>0</v>
       </c>
       <c r="N14" s="12"/>
-      <c r="O14" s="111"/>
-      <c r="P14" s="112"/>
-      <c r="Q14" s="112"/>
+      <c r="O14" s="130"/>
+      <c r="P14" s="131"/>
+      <c r="Q14" s="131"/>
       <c r="R14" s="52"/>
       <c r="S14" s="53"/>
       <c r="T14" s="53"/>
@@ -2839,7 +2839,7 @@
     </row>
     <row r="15" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="37">
-        <v>44701</v>
+        <v>44715</v>
       </c>
       <c r="C15" s="20" t="str">
         <f t="shared" si="0"/>
@@ -2861,9 +2861,9 @@
         <v>0</v>
       </c>
       <c r="N15" s="12"/>
-      <c r="O15" s="86"/>
-      <c r="P15" s="87"/>
-      <c r="Q15" s="87"/>
+      <c r="O15" s="132"/>
+      <c r="P15" s="133"/>
+      <c r="Q15" s="133"/>
       <c r="R15" s="52"/>
       <c r="S15" s="53"/>
       <c r="T15" s="53"/>
@@ -2875,7 +2875,7 @@
     </row>
     <row r="16" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="37">
-        <v>44702</v>
+        <v>44716</v>
       </c>
       <c r="C16" s="20" t="str">
         <f t="shared" si="0"/>
@@ -2897,9 +2897,9 @@
         <v>0</v>
       </c>
       <c r="N16" s="12"/>
-      <c r="O16" s="111"/>
-      <c r="P16" s="112"/>
-      <c r="Q16" s="112"/>
+      <c r="O16" s="130"/>
+      <c r="P16" s="131"/>
+      <c r="Q16" s="131"/>
       <c r="R16" s="52"/>
       <c r="S16" s="53"/>
       <c r="T16" s="53"/>
@@ -2911,7 +2911,7 @@
     </row>
     <row r="17" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="37">
-        <v>44703</v>
+        <v>44717</v>
       </c>
       <c r="C17" s="20" t="str">
         <f t="shared" si="0"/>
@@ -2933,9 +2933,9 @@
         <v>0</v>
       </c>
       <c r="N17" s="12"/>
-      <c r="O17" s="111"/>
-      <c r="P17" s="112"/>
-      <c r="Q17" s="112"/>
+      <c r="O17" s="130"/>
+      <c r="P17" s="131"/>
+      <c r="Q17" s="131"/>
       <c r="R17" s="52"/>
       <c r="S17" s="53"/>
       <c r="T17" s="53"/>
@@ -2965,9 +2965,9 @@
         <v>0</v>
       </c>
       <c r="N18" s="12"/>
-      <c r="O18" s="86"/>
-      <c r="P18" s="87"/>
-      <c r="Q18" s="113"/>
+      <c r="O18" s="132"/>
+      <c r="P18" s="133"/>
+      <c r="Q18" s="134"/>
       <c r="R18" s="52"/>
       <c r="S18" s="53"/>
       <c r="T18" s="53"/>
@@ -2997,9 +2997,9 @@
         <v>0</v>
       </c>
       <c r="N19" s="12"/>
-      <c r="O19" s="86"/>
-      <c r="P19" s="87"/>
-      <c r="Q19" s="113"/>
+      <c r="O19" s="132"/>
+      <c r="P19" s="133"/>
+      <c r="Q19" s="134"/>
       <c r="R19" s="52"/>
       <c r="S19" s="53"/>
       <c r="T19" s="53"/>
@@ -3029,9 +3029,9 @@
         <v>0</v>
       </c>
       <c r="N20" s="12"/>
-      <c r="O20" s="86"/>
-      <c r="P20" s="87"/>
-      <c r="Q20" s="113"/>
+      <c r="O20" s="132"/>
+      <c r="P20" s="133"/>
+      <c r="Q20" s="134"/>
       <c r="R20" s="52"/>
       <c r="S20" s="53"/>
       <c r="T20" s="53"/>
@@ -3061,9 +3061,9 @@
         <v>0</v>
       </c>
       <c r="N21" s="12"/>
-      <c r="O21" s="86"/>
-      <c r="P21" s="87"/>
-      <c r="Q21" s="113"/>
+      <c r="O21" s="132"/>
+      <c r="P21" s="133"/>
+      <c r="Q21" s="134"/>
       <c r="R21" s="52"/>
       <c r="S21" s="53"/>
       <c r="T21" s="53"/>
@@ -3093,9 +3093,9 @@
         <v>0</v>
       </c>
       <c r="N22" s="12"/>
-      <c r="O22" s="86"/>
-      <c r="P22" s="87"/>
-      <c r="Q22" s="113"/>
+      <c r="O22" s="132"/>
+      <c r="P22" s="133"/>
+      <c r="Q22" s="134"/>
       <c r="R22" s="52"/>
       <c r="S22" s="53"/>
       <c r="T22" s="53"/>
@@ -3125,9 +3125,9 @@
         <v>0</v>
       </c>
       <c r="N23" s="12"/>
-      <c r="O23" s="111"/>
-      <c r="P23" s="112"/>
-      <c r="Q23" s="112"/>
+      <c r="O23" s="130"/>
+      <c r="P23" s="131"/>
+      <c r="Q23" s="131"/>
       <c r="R23" s="52"/>
       <c r="S23" s="53"/>
       <c r="T23" s="53"/>
@@ -3157,9 +3157,9 @@
         <v>0</v>
       </c>
       <c r="N24" s="12"/>
-      <c r="O24" s="111"/>
-      <c r="P24" s="112"/>
-      <c r="Q24" s="112"/>
+      <c r="O24" s="130"/>
+      <c r="P24" s="131"/>
+      <c r="Q24" s="131"/>
       <c r="R24" s="52"/>
       <c r="S24" s="53"/>
       <c r="T24" s="53"/>
@@ -3338,25 +3338,25 @@
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
       <c r="H32" s="9"/>
-      <c r="I32" s="133" t="s">
+      <c r="I32" s="110" t="s">
         <v>68</v>
       </c>
-      <c r="J32" s="133"/>
-      <c r="K32" s="133"/>
-      <c r="L32" s="133"/>
-      <c r="M32" s="133"/>
-      <c r="N32" s="133"/>
-      <c r="O32" s="133"/>
+      <c r="J32" s="110"/>
+      <c r="K32" s="110"/>
+      <c r="L32" s="110"/>
+      <c r="M32" s="110"/>
+      <c r="N32" s="110"/>
+      <c r="O32" s="110"/>
       <c r="P32" s="10"/>
-      <c r="Q32" s="133" t="s">
+      <c r="Q32" s="110" t="s">
         <v>69</v>
       </c>
-      <c r="R32" s="133"/>
-      <c r="T32" s="133" t="s">
+      <c r="R32" s="110"/>
+      <c r="T32" s="110" t="s">
         <v>13</v>
       </c>
-      <c r="U32" s="133"/>
-      <c r="V32" s="133"/>
+      <c r="U32" s="110"/>
+      <c r="V32" s="110"/>
       <c r="AC32" t="s">
         <v>70</v>
       </c>
@@ -3395,27 +3395,27 @@
       </c>
     </row>
     <row r="35" spans="2:29" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="134"/>
-      <c r="C35" s="135"/>
-      <c r="D35" s="135"/>
-      <c r="E35" s="135"/>
-      <c r="F35" s="135"/>
-      <c r="G35" s="135"/>
-      <c r="H35" s="135"/>
-      <c r="I35" s="135"/>
-      <c r="J35" s="135"/>
-      <c r="K35" s="135"/>
-      <c r="L35" s="135"/>
-      <c r="M35" s="135"/>
-      <c r="N35" s="135"/>
-      <c r="O35" s="135"/>
-      <c r="P35" s="135"/>
-      <c r="Q35" s="135"/>
-      <c r="R35" s="135"/>
-      <c r="S35" s="135"/>
-      <c r="T35" s="135"/>
-      <c r="U35" s="135"/>
-      <c r="V35" s="136"/>
+      <c r="B35" s="111"/>
+      <c r="C35" s="112"/>
+      <c r="D35" s="112"/>
+      <c r="E35" s="112"/>
+      <c r="F35" s="112"/>
+      <c r="G35" s="112"/>
+      <c r="H35" s="112"/>
+      <c r="I35" s="112"/>
+      <c r="J35" s="112"/>
+      <c r="K35" s="112"/>
+      <c r="L35" s="112"/>
+      <c r="M35" s="112"/>
+      <c r="N35" s="112"/>
+      <c r="O35" s="112"/>
+      <c r="P35" s="112"/>
+      <c r="Q35" s="112"/>
+      <c r="R35" s="112"/>
+      <c r="S35" s="112"/>
+      <c r="T35" s="112"/>
+      <c r="U35" s="112"/>
+      <c r="V35" s="113"/>
       <c r="W35" s="36" t="s">
         <v>74</v>
       </c>
@@ -3435,29 +3435,29 @@
       </c>
     </row>
     <row r="37" spans="2:29" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B37" s="147" t="s">
+      <c r="B37" s="102" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="147"/>
-      <c r="D37" s="147"/>
-      <c r="E37" s="147"/>
-      <c r="F37" s="147"/>
-      <c r="G37" s="147"/>
-      <c r="H37" s="147"/>
-      <c r="I37" s="147"/>
-      <c r="J37" s="147"/>
-      <c r="K37" s="147"/>
-      <c r="L37" s="147"/>
-      <c r="M37" s="147"/>
-      <c r="N37" s="147"/>
-      <c r="O37" s="147"/>
-      <c r="P37" s="147"/>
-      <c r="Q37" s="147"/>
-      <c r="R37" s="147"/>
-      <c r="S37" s="147"/>
-      <c r="T37" s="147"/>
-      <c r="U37" s="147"/>
-      <c r="V37" s="147"/>
+      <c r="C37" s="102"/>
+      <c r="D37" s="102"/>
+      <c r="E37" s="102"/>
+      <c r="F37" s="102"/>
+      <c r="G37" s="102"/>
+      <c r="H37" s="102"/>
+      <c r="I37" s="102"/>
+      <c r="J37" s="102"/>
+      <c r="K37" s="102"/>
+      <c r="L37" s="102"/>
+      <c r="M37" s="102"/>
+      <c r="N37" s="102"/>
+      <c r="O37" s="102"/>
+      <c r="P37" s="102"/>
+      <c r="Q37" s="102"/>
+      <c r="R37" s="102"/>
+      <c r="S37" s="102"/>
+      <c r="T37" s="102"/>
+      <c r="U37" s="102"/>
+      <c r="V37" s="102"/>
       <c r="W37" s="30"/>
       <c r="X37" s="31"/>
       <c r="AC37" t="s">
@@ -3465,29 +3465,29 @@
       </c>
     </row>
     <row r="38" spans="2:29" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B38" s="148" t="s">
+      <c r="B38" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="148"/>
-      <c r="D38" s="148"/>
-      <c r="E38" s="148"/>
-      <c r="F38" s="148"/>
-      <c r="G38" s="148"/>
-      <c r="H38" s="148"/>
-      <c r="I38" s="148"/>
-      <c r="J38" s="148"/>
-      <c r="K38" s="148"/>
-      <c r="L38" s="148"/>
-      <c r="M38" s="148"/>
-      <c r="N38" s="148"/>
-      <c r="O38" s="148"/>
-      <c r="P38" s="148"/>
-      <c r="Q38" s="148"/>
-      <c r="R38" s="148"/>
-      <c r="S38" s="148"/>
-      <c r="T38" s="148"/>
-      <c r="U38" s="148"/>
-      <c r="V38" s="148"/>
+      <c r="C38" s="103"/>
+      <c r="D38" s="103"/>
+      <c r="E38" s="103"/>
+      <c r="F38" s="103"/>
+      <c r="G38" s="103"/>
+      <c r="H38" s="103"/>
+      <c r="I38" s="103"/>
+      <c r="J38" s="103"/>
+      <c r="K38" s="103"/>
+      <c r="L38" s="103"/>
+      <c r="M38" s="103"/>
+      <c r="N38" s="103"/>
+      <c r="O38" s="103"/>
+      <c r="P38" s="103"/>
+      <c r="Q38" s="103"/>
+      <c r="R38" s="103"/>
+      <c r="S38" s="103"/>
+      <c r="T38" s="103"/>
+      <c r="U38" s="103"/>
+      <c r="V38" s="103"/>
       <c r="W38" s="32"/>
       <c r="X38" s="32"/>
       <c r="AC38" t="s">
@@ -3503,28 +3503,28 @@
       <c r="B40" s="33">
         <v>1</v>
       </c>
-      <c r="C40" s="149" t="s">
+      <c r="C40" s="104" t="s">
         <v>82</v>
       </c>
-      <c r="D40" s="149"/>
-      <c r="E40" s="149"/>
-      <c r="F40" s="149"/>
-      <c r="G40" s="149"/>
-      <c r="H40" s="149"/>
-      <c r="I40" s="149"/>
-      <c r="J40" s="149"/>
-      <c r="K40" s="149"/>
-      <c r="L40" s="149"/>
-      <c r="M40" s="149"/>
-      <c r="N40" s="149"/>
-      <c r="O40" s="149"/>
-      <c r="P40" s="149"/>
-      <c r="Q40" s="149"/>
-      <c r="R40" s="149"/>
-      <c r="S40" s="149"/>
-      <c r="T40" s="149"/>
-      <c r="U40" s="149"/>
-      <c r="V40" s="149"/>
+      <c r="D40" s="104"/>
+      <c r="E40" s="104"/>
+      <c r="F40" s="104"/>
+      <c r="G40" s="104"/>
+      <c r="H40" s="104"/>
+      <c r="I40" s="104"/>
+      <c r="J40" s="104"/>
+      <c r="K40" s="104"/>
+      <c r="L40" s="104"/>
+      <c r="M40" s="104"/>
+      <c r="N40" s="104"/>
+      <c r="O40" s="104"/>
+      <c r="P40" s="104"/>
+      <c r="Q40" s="104"/>
+      <c r="R40" s="104"/>
+      <c r="S40" s="104"/>
+      <c r="T40" s="104"/>
+      <c r="U40" s="104"/>
+      <c r="V40" s="104"/>
       <c r="AC40" t="s">
         <v>83</v>
       </c>
@@ -3533,28 +3533,28 @@
       <c r="B41" s="33">
         <v>2</v>
       </c>
-      <c r="C41" s="149" t="s">
+      <c r="C41" s="104" t="s">
         <v>84</v>
       </c>
-      <c r="D41" s="149"/>
-      <c r="E41" s="149"/>
-      <c r="F41" s="149"/>
-      <c r="G41" s="149"/>
-      <c r="H41" s="149"/>
-      <c r="I41" s="149"/>
-      <c r="J41" s="149"/>
-      <c r="K41" s="149"/>
-      <c r="L41" s="149"/>
-      <c r="M41" s="149"/>
-      <c r="N41" s="149"/>
-      <c r="O41" s="149"/>
-      <c r="P41" s="149"/>
-      <c r="Q41" s="149"/>
-      <c r="R41" s="149"/>
-      <c r="S41" s="149"/>
-      <c r="T41" s="149"/>
-      <c r="U41" s="149"/>
-      <c r="V41" s="149"/>
+      <c r="D41" s="104"/>
+      <c r="E41" s="104"/>
+      <c r="F41" s="104"/>
+      <c r="G41" s="104"/>
+      <c r="H41" s="104"/>
+      <c r="I41" s="104"/>
+      <c r="J41" s="104"/>
+      <c r="K41" s="104"/>
+      <c r="L41" s="104"/>
+      <c r="M41" s="104"/>
+      <c r="N41" s="104"/>
+      <c r="O41" s="104"/>
+      <c r="P41" s="104"/>
+      <c r="Q41" s="104"/>
+      <c r="R41" s="104"/>
+      <c r="S41" s="104"/>
+      <c r="T41" s="104"/>
+      <c r="U41" s="104"/>
+      <c r="V41" s="104"/>
       <c r="AC41" t="s">
         <v>85</v>
       </c>
@@ -3563,28 +3563,28 @@
       <c r="B42" s="33">
         <v>3</v>
       </c>
-      <c r="C42" s="150" t="s">
+      <c r="C42" s="105" t="s">
         <v>86</v>
       </c>
-      <c r="D42" s="150"/>
-      <c r="E42" s="150"/>
-      <c r="F42" s="150"/>
-      <c r="G42" s="150"/>
-      <c r="H42" s="150"/>
-      <c r="I42" s="150"/>
-      <c r="J42" s="150"/>
-      <c r="K42" s="150"/>
-      <c r="L42" s="150"/>
-      <c r="M42" s="150"/>
-      <c r="N42" s="150"/>
-      <c r="O42" s="150"/>
-      <c r="P42" s="150"/>
-      <c r="Q42" s="150"/>
-      <c r="R42" s="150"/>
-      <c r="S42" s="150"/>
-      <c r="T42" s="150"/>
-      <c r="U42" s="150"/>
-      <c r="V42" s="150"/>
+      <c r="D42" s="105"/>
+      <c r="E42" s="105"/>
+      <c r="F42" s="105"/>
+      <c r="G42" s="105"/>
+      <c r="H42" s="105"/>
+      <c r="I42" s="105"/>
+      <c r="J42" s="105"/>
+      <c r="K42" s="105"/>
+      <c r="L42" s="105"/>
+      <c r="M42" s="105"/>
+      <c r="N42" s="105"/>
+      <c r="O42" s="105"/>
+      <c r="P42" s="105"/>
+      <c r="Q42" s="105"/>
+      <c r="R42" s="105"/>
+      <c r="S42" s="105"/>
+      <c r="T42" s="105"/>
+      <c r="U42" s="105"/>
+      <c r="V42" s="105"/>
       <c r="AC42" t="s">
         <v>87</v>
       </c>
@@ -3593,28 +3593,28 @@
       <c r="B43" s="33">
         <v>4</v>
       </c>
-      <c r="C43" s="149" t="s">
+      <c r="C43" s="104" t="s">
         <v>88</v>
       </c>
-      <c r="D43" s="149"/>
-      <c r="E43" s="149"/>
-      <c r="F43" s="149"/>
-      <c r="G43" s="149"/>
-      <c r="H43" s="149"/>
-      <c r="I43" s="149"/>
-      <c r="J43" s="149"/>
-      <c r="K43" s="149"/>
-      <c r="L43" s="149"/>
-      <c r="M43" s="149"/>
-      <c r="N43" s="149"/>
-      <c r="O43" s="149"/>
-      <c r="P43" s="149"/>
-      <c r="Q43" s="149"/>
-      <c r="R43" s="149"/>
-      <c r="S43" s="149"/>
-      <c r="T43" s="149"/>
-      <c r="U43" s="149"/>
-      <c r="V43" s="149"/>
+      <c r="D43" s="104"/>
+      <c r="E43" s="104"/>
+      <c r="F43" s="104"/>
+      <c r="G43" s="104"/>
+      <c r="H43" s="104"/>
+      <c r="I43" s="104"/>
+      <c r="J43" s="104"/>
+      <c r="K43" s="104"/>
+      <c r="L43" s="104"/>
+      <c r="M43" s="104"/>
+      <c r="N43" s="104"/>
+      <c r="O43" s="104"/>
+      <c r="P43" s="104"/>
+      <c r="Q43" s="104"/>
+      <c r="R43" s="104"/>
+      <c r="S43" s="104"/>
+      <c r="T43" s="104"/>
+      <c r="U43" s="104"/>
+      <c r="V43" s="104"/>
       <c r="AC43" t="s">
         <v>89</v>
       </c>
@@ -3623,28 +3623,28 @@
       <c r="B44" s="33">
         <v>5</v>
       </c>
-      <c r="C44" s="149" t="s">
+      <c r="C44" s="104" t="s">
         <v>90</v>
       </c>
-      <c r="D44" s="149"/>
-      <c r="E44" s="149"/>
-      <c r="F44" s="149"/>
-      <c r="G44" s="149"/>
-      <c r="H44" s="149"/>
-      <c r="I44" s="149"/>
-      <c r="J44" s="149"/>
-      <c r="K44" s="149"/>
-      <c r="L44" s="149"/>
-      <c r="M44" s="149"/>
-      <c r="N44" s="149"/>
-      <c r="O44" s="149"/>
-      <c r="P44" s="149"/>
-      <c r="Q44" s="149"/>
-      <c r="R44" s="149"/>
-      <c r="S44" s="149"/>
-      <c r="T44" s="149"/>
-      <c r="U44" s="149"/>
-      <c r="V44" s="149"/>
+      <c r="D44" s="104"/>
+      <c r="E44" s="104"/>
+      <c r="F44" s="104"/>
+      <c r="G44" s="104"/>
+      <c r="H44" s="104"/>
+      <c r="I44" s="104"/>
+      <c r="J44" s="104"/>
+      <c r="K44" s="104"/>
+      <c r="L44" s="104"/>
+      <c r="M44" s="104"/>
+      <c r="N44" s="104"/>
+      <c r="O44" s="104"/>
+      <c r="P44" s="104"/>
+      <c r="Q44" s="104"/>
+      <c r="R44" s="104"/>
+      <c r="S44" s="104"/>
+      <c r="T44" s="104"/>
+      <c r="U44" s="104"/>
+      <c r="V44" s="104"/>
       <c r="AC44" t="s">
         <v>91</v>
       </c>
@@ -3653,28 +3653,28 @@
       <c r="B45" s="33">
         <v>6</v>
       </c>
-      <c r="C45" s="149" t="s">
+      <c r="C45" s="104" t="s">
         <v>92</v>
       </c>
-      <c r="D45" s="149"/>
-      <c r="E45" s="149"/>
-      <c r="F45" s="149"/>
-      <c r="G45" s="149"/>
-      <c r="H45" s="149"/>
-      <c r="I45" s="149"/>
-      <c r="J45" s="149"/>
-      <c r="K45" s="149"/>
-      <c r="L45" s="149"/>
-      <c r="M45" s="149"/>
-      <c r="N45" s="149"/>
-      <c r="O45" s="149"/>
-      <c r="P45" s="149"/>
-      <c r="Q45" s="149"/>
-      <c r="R45" s="149"/>
-      <c r="S45" s="149"/>
-      <c r="T45" s="149"/>
-      <c r="U45" s="149"/>
-      <c r="V45" s="149"/>
+      <c r="D45" s="104"/>
+      <c r="E45" s="104"/>
+      <c r="F45" s="104"/>
+      <c r="G45" s="104"/>
+      <c r="H45" s="104"/>
+      <c r="I45" s="104"/>
+      <c r="J45" s="104"/>
+      <c r="K45" s="104"/>
+      <c r="L45" s="104"/>
+      <c r="M45" s="104"/>
+      <c r="N45" s="104"/>
+      <c r="O45" s="104"/>
+      <c r="P45" s="104"/>
+      <c r="Q45" s="104"/>
+      <c r="R45" s="104"/>
+      <c r="S45" s="104"/>
+      <c r="T45" s="104"/>
+      <c r="U45" s="104"/>
+      <c r="V45" s="104"/>
       <c r="AC45" t="s">
         <v>93</v>
       </c>
@@ -3683,28 +3683,28 @@
       <c r="B46" s="33">
         <v>7</v>
       </c>
-      <c r="C46" s="149" t="s">
+      <c r="C46" s="104" t="s">
         <v>94</v>
       </c>
-      <c r="D46" s="149"/>
-      <c r="E46" s="149"/>
-      <c r="F46" s="149"/>
-      <c r="G46" s="149"/>
-      <c r="H46" s="149"/>
-      <c r="I46" s="149"/>
-      <c r="J46" s="149"/>
-      <c r="K46" s="149"/>
-      <c r="L46" s="149"/>
-      <c r="M46" s="149"/>
-      <c r="N46" s="149"/>
-      <c r="O46" s="149"/>
-      <c r="P46" s="149"/>
-      <c r="Q46" s="149"/>
-      <c r="R46" s="149"/>
-      <c r="S46" s="149"/>
-      <c r="T46" s="149"/>
-      <c r="U46" s="149"/>
-      <c r="V46" s="149"/>
+      <c r="D46" s="104"/>
+      <c r="E46" s="104"/>
+      <c r="F46" s="104"/>
+      <c r="G46" s="104"/>
+      <c r="H46" s="104"/>
+      <c r="I46" s="104"/>
+      <c r="J46" s="104"/>
+      <c r="K46" s="104"/>
+      <c r="L46" s="104"/>
+      <c r="M46" s="104"/>
+      <c r="N46" s="104"/>
+      <c r="O46" s="104"/>
+      <c r="P46" s="104"/>
+      <c r="Q46" s="104"/>
+      <c r="R46" s="104"/>
+      <c r="S46" s="104"/>
+      <c r="T46" s="104"/>
+      <c r="U46" s="104"/>
+      <c r="V46" s="104"/>
       <c r="AC46" t="s">
         <v>95</v>
       </c>
@@ -3713,28 +3713,28 @@
       <c r="B47" s="70">
         <v>8</v>
       </c>
-      <c r="C47" s="137" t="s">
+      <c r="C47" s="106" t="s">
         <v>96</v>
       </c>
-      <c r="D47" s="149"/>
-      <c r="E47" s="149"/>
-      <c r="F47" s="149"/>
-      <c r="G47" s="149"/>
-      <c r="H47" s="149"/>
-      <c r="I47" s="149"/>
-      <c r="J47" s="149"/>
-      <c r="K47" s="149"/>
-      <c r="L47" s="149"/>
-      <c r="M47" s="149"/>
-      <c r="N47" s="149"/>
-      <c r="O47" s="149"/>
-      <c r="P47" s="149"/>
-      <c r="Q47" s="149"/>
-      <c r="R47" s="149"/>
-      <c r="S47" s="149"/>
-      <c r="T47" s="149"/>
-      <c r="U47" s="149"/>
-      <c r="V47" s="149"/>
+      <c r="D47" s="104"/>
+      <c r="E47" s="104"/>
+      <c r="F47" s="104"/>
+      <c r="G47" s="104"/>
+      <c r="H47" s="104"/>
+      <c r="I47" s="104"/>
+      <c r="J47" s="104"/>
+      <c r="K47" s="104"/>
+      <c r="L47" s="104"/>
+      <c r="M47" s="104"/>
+      <c r="N47" s="104"/>
+      <c r="O47" s="104"/>
+      <c r="P47" s="104"/>
+      <c r="Q47" s="104"/>
+      <c r="R47" s="104"/>
+      <c r="S47" s="104"/>
+      <c r="T47" s="104"/>
+      <c r="U47" s="104"/>
+      <c r="V47" s="104"/>
       <c r="AC47" t="s">
         <v>97</v>
       </c>
@@ -3743,28 +3743,28 @@
       <c r="B48" s="70">
         <v>9</v>
       </c>
-      <c r="C48" s="137" t="s">
+      <c r="C48" s="106" t="s">
         <v>98</v>
       </c>
-      <c r="D48" s="137"/>
-      <c r="E48" s="137"/>
-      <c r="F48" s="137"/>
-      <c r="G48" s="137"/>
-      <c r="H48" s="137"/>
-      <c r="I48" s="137"/>
-      <c r="J48" s="137"/>
-      <c r="K48" s="137"/>
-      <c r="L48" s="137"/>
-      <c r="M48" s="137"/>
-      <c r="N48" s="137"/>
-      <c r="O48" s="137"/>
-      <c r="P48" s="137"/>
-      <c r="Q48" s="137"/>
-      <c r="R48" s="137"/>
-      <c r="S48" s="137"/>
-      <c r="T48" s="137"/>
-      <c r="U48" s="137"/>
-      <c r="V48" s="137"/>
+      <c r="D48" s="106"/>
+      <c r="E48" s="106"/>
+      <c r="F48" s="106"/>
+      <c r="G48" s="106"/>
+      <c r="H48" s="106"/>
+      <c r="I48" s="106"/>
+      <c r="J48" s="106"/>
+      <c r="K48" s="106"/>
+      <c r="L48" s="106"/>
+      <c r="M48" s="106"/>
+      <c r="N48" s="106"/>
+      <c r="O48" s="106"/>
+      <c r="P48" s="106"/>
+      <c r="Q48" s="106"/>
+      <c r="R48" s="106"/>
+      <c r="S48" s="106"/>
+      <c r="T48" s="106"/>
+      <c r="U48" s="106"/>
+      <c r="V48" s="106"/>
       <c r="AC48" t="s">
         <v>99</v>
       </c>
@@ -3773,28 +3773,28 @@
       <c r="B49" s="70">
         <v>10</v>
       </c>
-      <c r="C49" s="149" t="s">
+      <c r="C49" s="104" t="s">
         <v>100</v>
       </c>
-      <c r="D49" s="149"/>
-      <c r="E49" s="149"/>
-      <c r="F49" s="149"/>
-      <c r="G49" s="149"/>
-      <c r="H49" s="149"/>
-      <c r="I49" s="149"/>
-      <c r="J49" s="149"/>
-      <c r="K49" s="149"/>
-      <c r="L49" s="149"/>
-      <c r="M49" s="149"/>
-      <c r="N49" s="149"/>
-      <c r="O49" s="149"/>
-      <c r="P49" s="149"/>
-      <c r="Q49" s="149"/>
-      <c r="R49" s="149"/>
-      <c r="S49" s="149"/>
-      <c r="T49" s="149"/>
-      <c r="U49" s="149"/>
-      <c r="V49" s="149"/>
+      <c r="D49" s="104"/>
+      <c r="E49" s="104"/>
+      <c r="F49" s="104"/>
+      <c r="G49" s="104"/>
+      <c r="H49" s="104"/>
+      <c r="I49" s="104"/>
+      <c r="J49" s="104"/>
+      <c r="K49" s="104"/>
+      <c r="L49" s="104"/>
+      <c r="M49" s="104"/>
+      <c r="N49" s="104"/>
+      <c r="O49" s="104"/>
+      <c r="P49" s="104"/>
+      <c r="Q49" s="104"/>
+      <c r="R49" s="104"/>
+      <c r="S49" s="104"/>
+      <c r="T49" s="104"/>
+      <c r="U49" s="104"/>
+      <c r="V49" s="104"/>
       <c r="AC49" t="s">
         <v>101</v>
       </c>
@@ -3861,28 +3861,28 @@
       <c r="B52" s="70">
         <v>12</v>
       </c>
-      <c r="C52" s="149" t="s">
+      <c r="C52" s="104" t="s">
         <v>106</v>
       </c>
-      <c r="D52" s="149"/>
-      <c r="E52" s="149"/>
-      <c r="F52" s="149"/>
-      <c r="G52" s="149"/>
-      <c r="H52" s="149"/>
-      <c r="I52" s="149"/>
-      <c r="J52" s="149"/>
-      <c r="K52" s="149"/>
-      <c r="L52" s="149"/>
-      <c r="M52" s="149"/>
-      <c r="N52" s="149"/>
-      <c r="O52" s="149"/>
-      <c r="P52" s="149"/>
-      <c r="Q52" s="149"/>
-      <c r="R52" s="149"/>
-      <c r="S52" s="149"/>
-      <c r="T52" s="149"/>
-      <c r="U52" s="149"/>
-      <c r="V52" s="149"/>
+      <c r="D52" s="104"/>
+      <c r="E52" s="104"/>
+      <c r="F52" s="104"/>
+      <c r="G52" s="104"/>
+      <c r="H52" s="104"/>
+      <c r="I52" s="104"/>
+      <c r="J52" s="104"/>
+      <c r="K52" s="104"/>
+      <c r="L52" s="104"/>
+      <c r="M52" s="104"/>
+      <c r="N52" s="104"/>
+      <c r="O52" s="104"/>
+      <c r="P52" s="104"/>
+      <c r="Q52" s="104"/>
+      <c r="R52" s="104"/>
+      <c r="S52" s="104"/>
+      <c r="T52" s="104"/>
+      <c r="U52" s="104"/>
+      <c r="V52" s="104"/>
       <c r="AC52" t="s">
         <v>107</v>
       </c>
@@ -3898,406 +3898,406 @@
       </c>
     </row>
     <row r="54" spans="2:29" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="130" t="s">
+      <c r="B54" s="107" t="s">
         <v>109</v>
       </c>
-      <c r="C54" s="131"/>
-      <c r="D54" s="131"/>
-      <c r="E54" s="132"/>
-      <c r="F54" s="144" t="s">
+      <c r="C54" s="108"/>
+      <c r="D54" s="108"/>
+      <c r="E54" s="109"/>
+      <c r="F54" s="99" t="s">
         <v>110</v>
       </c>
-      <c r="G54" s="145"/>
-      <c r="H54" s="145"/>
-      <c r="I54" s="145"/>
-      <c r="J54" s="145"/>
-      <c r="K54" s="145"/>
-      <c r="L54" s="145"/>
-      <c r="M54" s="145"/>
-      <c r="N54" s="145"/>
-      <c r="O54" s="145"/>
-      <c r="P54" s="145"/>
-      <c r="Q54" s="145"/>
-      <c r="R54" s="145"/>
-      <c r="S54" s="145"/>
-      <c r="T54" s="145"/>
-      <c r="U54" s="145"/>
-      <c r="V54" s="146"/>
+      <c r="G54" s="100"/>
+      <c r="H54" s="100"/>
+      <c r="I54" s="100"/>
+      <c r="J54" s="100"/>
+      <c r="K54" s="100"/>
+      <c r="L54" s="100"/>
+      <c r="M54" s="100"/>
+      <c r="N54" s="100"/>
+      <c r="O54" s="100"/>
+      <c r="P54" s="100"/>
+      <c r="Q54" s="100"/>
+      <c r="R54" s="100"/>
+      <c r="S54" s="100"/>
+      <c r="T54" s="100"/>
+      <c r="U54" s="100"/>
+      <c r="V54" s="101"/>
       <c r="AC54" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="55" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B55" s="138" t="s">
+      <c r="B55" s="87" t="s">
         <v>112</v>
       </c>
-      <c r="C55" s="139"/>
-      <c r="D55" s="139"/>
-      <c r="E55" s="140"/>
-      <c r="F55" s="157" t="s">
+      <c r="C55" s="88"/>
+      <c r="D55" s="88"/>
+      <c r="E55" s="89"/>
+      <c r="F55" s="79" t="s">
         <v>113</v>
       </c>
-      <c r="G55" s="163"/>
-      <c r="H55" s="163"/>
-      <c r="I55" s="163"/>
-      <c r="J55" s="163"/>
-      <c r="K55" s="163"/>
-      <c r="L55" s="163"/>
-      <c r="M55" s="163"/>
-      <c r="N55" s="163"/>
-      <c r="O55" s="163"/>
-      <c r="P55" s="163"/>
-      <c r="Q55" s="163"/>
-      <c r="R55" s="163"/>
-      <c r="S55" s="163"/>
-      <c r="T55" s="163"/>
-      <c r="U55" s="163"/>
-      <c r="V55" s="164"/>
+      <c r="G55" s="80"/>
+      <c r="H55" s="80"/>
+      <c r="I55" s="80"/>
+      <c r="J55" s="80"/>
+      <c r="K55" s="80"/>
+      <c r="L55" s="80"/>
+      <c r="M55" s="80"/>
+      <c r="N55" s="80"/>
+      <c r="O55" s="80"/>
+      <c r="P55" s="80"/>
+      <c r="Q55" s="80"/>
+      <c r="R55" s="80"/>
+      <c r="S55" s="80"/>
+      <c r="T55" s="80"/>
+      <c r="U55" s="80"/>
+      <c r="V55" s="81"/>
       <c r="AC55" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="56" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B56" s="138" t="s">
+      <c r="B56" s="87" t="s">
         <v>115</v>
       </c>
-      <c r="C56" s="139"/>
-      <c r="D56" s="139"/>
-      <c r="E56" s="140"/>
-      <c r="F56" s="157" t="s">
+      <c r="C56" s="88"/>
+      <c r="D56" s="88"/>
+      <c r="E56" s="89"/>
+      <c r="F56" s="79" t="s">
         <v>116</v>
       </c>
-      <c r="G56" s="163"/>
-      <c r="H56" s="163"/>
-      <c r="I56" s="163"/>
-      <c r="J56" s="163"/>
-      <c r="K56" s="163"/>
-      <c r="L56" s="163"/>
-      <c r="M56" s="163"/>
-      <c r="N56" s="163"/>
-      <c r="O56" s="163"/>
-      <c r="P56" s="163"/>
-      <c r="Q56" s="163"/>
-      <c r="R56" s="163"/>
-      <c r="S56" s="163"/>
-      <c r="T56" s="163"/>
-      <c r="U56" s="163"/>
-      <c r="V56" s="164"/>
+      <c r="G56" s="80"/>
+      <c r="H56" s="80"/>
+      <c r="I56" s="80"/>
+      <c r="J56" s="80"/>
+      <c r="K56" s="80"/>
+      <c r="L56" s="80"/>
+      <c r="M56" s="80"/>
+      <c r="N56" s="80"/>
+      <c r="O56" s="80"/>
+      <c r="P56" s="80"/>
+      <c r="Q56" s="80"/>
+      <c r="R56" s="80"/>
+      <c r="S56" s="80"/>
+      <c r="T56" s="80"/>
+      <c r="U56" s="80"/>
+      <c r="V56" s="81"/>
       <c r="AC56" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="57" spans="2:29" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="138" t="s">
+      <c r="B57" s="87" t="s">
         <v>118</v>
       </c>
-      <c r="C57" s="139"/>
-      <c r="D57" s="139"/>
-      <c r="E57" s="140"/>
-      <c r="F57" s="141" t="s">
+      <c r="C57" s="88"/>
+      <c r="D57" s="88"/>
+      <c r="E57" s="89"/>
+      <c r="F57" s="96" t="s">
         <v>119</v>
       </c>
-      <c r="G57" s="142"/>
-      <c r="H57" s="142"/>
-      <c r="I57" s="142"/>
-      <c r="J57" s="142"/>
-      <c r="K57" s="142"/>
-      <c r="L57" s="142"/>
-      <c r="M57" s="142"/>
-      <c r="N57" s="142"/>
-      <c r="O57" s="142"/>
-      <c r="P57" s="142"/>
-      <c r="Q57" s="142"/>
-      <c r="R57" s="142"/>
-      <c r="S57" s="142"/>
-      <c r="T57" s="142"/>
-      <c r="U57" s="142"/>
-      <c r="V57" s="143"/>
+      <c r="G57" s="97"/>
+      <c r="H57" s="97"/>
+      <c r="I57" s="97"/>
+      <c r="J57" s="97"/>
+      <c r="K57" s="97"/>
+      <c r="L57" s="97"/>
+      <c r="M57" s="97"/>
+      <c r="N57" s="97"/>
+      <c r="O57" s="97"/>
+      <c r="P57" s="97"/>
+      <c r="Q57" s="97"/>
+      <c r="R57" s="97"/>
+      <c r="S57" s="97"/>
+      <c r="T57" s="97"/>
+      <c r="U57" s="97"/>
+      <c r="V57" s="98"/>
       <c r="AC57" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="58" spans="2:29" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="138" t="s">
+      <c r="B58" s="87" t="s">
         <v>121</v>
       </c>
-      <c r="C58" s="139"/>
-      <c r="D58" s="139"/>
-      <c r="E58" s="140"/>
-      <c r="F58" s="141" t="s">
+      <c r="C58" s="88"/>
+      <c r="D58" s="88"/>
+      <c r="E58" s="89"/>
+      <c r="F58" s="96" t="s">
         <v>122</v>
       </c>
-      <c r="G58" s="142"/>
-      <c r="H58" s="142"/>
-      <c r="I58" s="142"/>
-      <c r="J58" s="142"/>
-      <c r="K58" s="142"/>
-      <c r="L58" s="142"/>
-      <c r="M58" s="142"/>
-      <c r="N58" s="142"/>
-      <c r="O58" s="142"/>
-      <c r="P58" s="142"/>
-      <c r="Q58" s="142"/>
-      <c r="R58" s="142"/>
-      <c r="S58" s="142"/>
-      <c r="T58" s="142"/>
-      <c r="U58" s="142"/>
-      <c r="V58" s="143"/>
+      <c r="G58" s="97"/>
+      <c r="H58" s="97"/>
+      <c r="I58" s="97"/>
+      <c r="J58" s="97"/>
+      <c r="K58" s="97"/>
+      <c r="L58" s="97"/>
+      <c r="M58" s="97"/>
+      <c r="N58" s="97"/>
+      <c r="O58" s="97"/>
+      <c r="P58" s="97"/>
+      <c r="Q58" s="97"/>
+      <c r="R58" s="97"/>
+      <c r="S58" s="97"/>
+      <c r="T58" s="97"/>
+      <c r="U58" s="97"/>
+      <c r="V58" s="98"/>
       <c r="AC58" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="59" spans="2:29" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="151" t="s">
+      <c r="B59" s="73" t="s">
         <v>124</v>
       </c>
-      <c r="C59" s="152"/>
-      <c r="D59" s="152"/>
-      <c r="E59" s="153"/>
-      <c r="F59" s="167" t="s">
+      <c r="C59" s="74"/>
+      <c r="D59" s="74"/>
+      <c r="E59" s="75"/>
+      <c r="F59" s="84" t="s">
         <v>125</v>
       </c>
-      <c r="G59" s="168"/>
-      <c r="H59" s="168"/>
-      <c r="I59" s="168"/>
-      <c r="J59" s="168"/>
-      <c r="K59" s="168"/>
-      <c r="L59" s="168"/>
-      <c r="M59" s="168"/>
-      <c r="N59" s="168"/>
-      <c r="O59" s="168"/>
-      <c r="P59" s="168"/>
-      <c r="Q59" s="168"/>
-      <c r="R59" s="168"/>
-      <c r="S59" s="168"/>
-      <c r="T59" s="168"/>
-      <c r="U59" s="168"/>
-      <c r="V59" s="169"/>
+      <c r="G59" s="85"/>
+      <c r="H59" s="85"/>
+      <c r="I59" s="85"/>
+      <c r="J59" s="85"/>
+      <c r="K59" s="85"/>
+      <c r="L59" s="85"/>
+      <c r="M59" s="85"/>
+      <c r="N59" s="85"/>
+      <c r="O59" s="85"/>
+      <c r="P59" s="85"/>
+      <c r="Q59" s="85"/>
+      <c r="R59" s="85"/>
+      <c r="S59" s="85"/>
+      <c r="T59" s="85"/>
+      <c r="U59" s="85"/>
+      <c r="V59" s="86"/>
       <c r="AC59" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="60" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B60" s="138" t="s">
+      <c r="B60" s="87" t="s">
         <v>127</v>
       </c>
-      <c r="C60" s="139"/>
-      <c r="D60" s="139"/>
-      <c r="E60" s="140"/>
-      <c r="F60" s="157" t="s">
+      <c r="C60" s="88"/>
+      <c r="D60" s="88"/>
+      <c r="E60" s="89"/>
+      <c r="F60" s="79" t="s">
         <v>128</v>
       </c>
-      <c r="G60" s="158"/>
-      <c r="H60" s="158"/>
-      <c r="I60" s="158"/>
-      <c r="J60" s="158"/>
-      <c r="K60" s="158"/>
-      <c r="L60" s="158"/>
-      <c r="M60" s="158"/>
-      <c r="N60" s="158"/>
-      <c r="O60" s="158"/>
-      <c r="P60" s="158"/>
-      <c r="Q60" s="158"/>
-      <c r="R60" s="158"/>
-      <c r="S60" s="158"/>
-      <c r="T60" s="158"/>
-      <c r="U60" s="158"/>
-      <c r="V60" s="159"/>
+      <c r="G60" s="82"/>
+      <c r="H60" s="82"/>
+      <c r="I60" s="82"/>
+      <c r="J60" s="82"/>
+      <c r="K60" s="82"/>
+      <c r="L60" s="82"/>
+      <c r="M60" s="82"/>
+      <c r="N60" s="82"/>
+      <c r="O60" s="82"/>
+      <c r="P60" s="82"/>
+      <c r="Q60" s="82"/>
+      <c r="R60" s="82"/>
+      <c r="S60" s="82"/>
+      <c r="T60" s="82"/>
+      <c r="U60" s="82"/>
+      <c r="V60" s="83"/>
       <c r="AC60" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="61" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B61" s="138" t="s">
+      <c r="B61" s="87" t="s">
         <v>130</v>
       </c>
-      <c r="C61" s="139"/>
-      <c r="D61" s="139"/>
-      <c r="E61" s="140"/>
-      <c r="F61" s="157" t="s">
+      <c r="C61" s="88"/>
+      <c r="D61" s="88"/>
+      <c r="E61" s="89"/>
+      <c r="F61" s="79" t="s">
         <v>131</v>
       </c>
-      <c r="G61" s="163"/>
-      <c r="H61" s="163"/>
-      <c r="I61" s="163"/>
-      <c r="J61" s="163"/>
-      <c r="K61" s="163"/>
-      <c r="L61" s="163"/>
-      <c r="M61" s="163"/>
-      <c r="N61" s="163"/>
-      <c r="O61" s="163"/>
-      <c r="P61" s="163"/>
-      <c r="Q61" s="163"/>
-      <c r="R61" s="163"/>
-      <c r="S61" s="163"/>
-      <c r="T61" s="163"/>
-      <c r="U61" s="163"/>
-      <c r="V61" s="164"/>
+      <c r="G61" s="80"/>
+      <c r="H61" s="80"/>
+      <c r="I61" s="80"/>
+      <c r="J61" s="80"/>
+      <c r="K61" s="80"/>
+      <c r="L61" s="80"/>
+      <c r="M61" s="80"/>
+      <c r="N61" s="80"/>
+      <c r="O61" s="80"/>
+      <c r="P61" s="80"/>
+      <c r="Q61" s="80"/>
+      <c r="R61" s="80"/>
+      <c r="S61" s="80"/>
+      <c r="T61" s="80"/>
+      <c r="U61" s="80"/>
+      <c r="V61" s="81"/>
       <c r="AC61" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="62" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B62" s="138" t="s">
+      <c r="B62" s="87" t="s">
         <v>133</v>
       </c>
-      <c r="C62" s="139"/>
-      <c r="D62" s="139"/>
-      <c r="E62" s="140"/>
-      <c r="F62" s="157" t="s">
+      <c r="C62" s="88"/>
+      <c r="D62" s="88"/>
+      <c r="E62" s="89"/>
+      <c r="F62" s="79" t="s">
         <v>134</v>
       </c>
-      <c r="G62" s="163"/>
-      <c r="H62" s="163"/>
-      <c r="I62" s="163"/>
-      <c r="J62" s="163"/>
-      <c r="K62" s="163"/>
-      <c r="L62" s="163"/>
-      <c r="M62" s="163"/>
-      <c r="N62" s="163"/>
-      <c r="O62" s="163"/>
-      <c r="P62" s="163"/>
-      <c r="Q62" s="163"/>
-      <c r="R62" s="163"/>
-      <c r="S62" s="163"/>
-      <c r="T62" s="163"/>
-      <c r="U62" s="163"/>
-      <c r="V62" s="164"/>
+      <c r="G62" s="80"/>
+      <c r="H62" s="80"/>
+      <c r="I62" s="80"/>
+      <c r="J62" s="80"/>
+      <c r="K62" s="80"/>
+      <c r="L62" s="80"/>
+      <c r="M62" s="80"/>
+      <c r="N62" s="80"/>
+      <c r="O62" s="80"/>
+      <c r="P62" s="80"/>
+      <c r="Q62" s="80"/>
+      <c r="R62" s="80"/>
+      <c r="S62" s="80"/>
+      <c r="T62" s="80"/>
+      <c r="U62" s="80"/>
+      <c r="V62" s="81"/>
     </row>
     <row r="63" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B63" s="151" t="s">
+      <c r="B63" s="73" t="s">
         <v>135</v>
       </c>
-      <c r="C63" s="152"/>
-      <c r="D63" s="152"/>
-      <c r="E63" s="153"/>
-      <c r="F63" s="157" t="s">
+      <c r="C63" s="74"/>
+      <c r="D63" s="74"/>
+      <c r="E63" s="75"/>
+      <c r="F63" s="79" t="s">
         <v>136</v>
       </c>
-      <c r="G63" s="163"/>
-      <c r="H63" s="163"/>
-      <c r="I63" s="163"/>
-      <c r="J63" s="163"/>
-      <c r="K63" s="163"/>
-      <c r="L63" s="163"/>
-      <c r="M63" s="163"/>
-      <c r="N63" s="163"/>
-      <c r="O63" s="163"/>
-      <c r="P63" s="163"/>
-      <c r="Q63" s="163"/>
-      <c r="R63" s="163"/>
-      <c r="S63" s="163"/>
-      <c r="T63" s="163"/>
-      <c r="U63" s="163"/>
-      <c r="V63" s="164"/>
+      <c r="G63" s="80"/>
+      <c r="H63" s="80"/>
+      <c r="I63" s="80"/>
+      <c r="J63" s="80"/>
+      <c r="K63" s="80"/>
+      <c r="L63" s="80"/>
+      <c r="M63" s="80"/>
+      <c r="N63" s="80"/>
+      <c r="O63" s="80"/>
+      <c r="P63" s="80"/>
+      <c r="Q63" s="80"/>
+      <c r="R63" s="80"/>
+      <c r="S63" s="80"/>
+      <c r="T63" s="80"/>
+      <c r="U63" s="80"/>
+      <c r="V63" s="81"/>
     </row>
     <row r="64" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B64" s="151" t="s">
+      <c r="B64" s="73" t="s">
         <v>137</v>
       </c>
-      <c r="C64" s="152"/>
-      <c r="D64" s="152"/>
-      <c r="E64" s="153"/>
-      <c r="F64" s="157" t="s">
+      <c r="C64" s="74"/>
+      <c r="D64" s="74"/>
+      <c r="E64" s="75"/>
+      <c r="F64" s="79" t="s">
         <v>138</v>
       </c>
-      <c r="G64" s="163"/>
-      <c r="H64" s="163"/>
-      <c r="I64" s="163"/>
-      <c r="J64" s="163"/>
-      <c r="K64" s="163"/>
-      <c r="L64" s="163"/>
-      <c r="M64" s="163"/>
-      <c r="N64" s="163"/>
-      <c r="O64" s="163"/>
-      <c r="P64" s="163"/>
-      <c r="Q64" s="163"/>
-      <c r="R64" s="163"/>
-      <c r="S64" s="163"/>
-      <c r="T64" s="163"/>
-      <c r="U64" s="163"/>
-      <c r="V64" s="164"/>
+      <c r="G64" s="80"/>
+      <c r="H64" s="80"/>
+      <c r="I64" s="80"/>
+      <c r="J64" s="80"/>
+      <c r="K64" s="80"/>
+      <c r="L64" s="80"/>
+      <c r="M64" s="80"/>
+      <c r="N64" s="80"/>
+      <c r="O64" s="80"/>
+      <c r="P64" s="80"/>
+      <c r="Q64" s="80"/>
+      <c r="R64" s="80"/>
+      <c r="S64" s="80"/>
+      <c r="T64" s="80"/>
+      <c r="U64" s="80"/>
+      <c r="V64" s="81"/>
     </row>
     <row r="65" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B65" s="151" t="s">
+      <c r="B65" s="73" t="s">
         <v>139</v>
       </c>
-      <c r="C65" s="152"/>
-      <c r="D65" s="152"/>
-      <c r="E65" s="153"/>
-      <c r="F65" s="157" t="s">
+      <c r="C65" s="74"/>
+      <c r="D65" s="74"/>
+      <c r="E65" s="75"/>
+      <c r="F65" s="79" t="s">
         <v>140</v>
       </c>
-      <c r="G65" s="158"/>
-      <c r="H65" s="158"/>
-      <c r="I65" s="158"/>
-      <c r="J65" s="158"/>
-      <c r="K65" s="158"/>
-      <c r="L65" s="158"/>
-      <c r="M65" s="158"/>
-      <c r="N65" s="158"/>
-      <c r="O65" s="158"/>
-      <c r="P65" s="158"/>
-      <c r="Q65" s="158"/>
-      <c r="R65" s="158"/>
-      <c r="S65" s="158"/>
-      <c r="T65" s="158"/>
-      <c r="U65" s="158"/>
-      <c r="V65" s="159"/>
+      <c r="G65" s="82"/>
+      <c r="H65" s="82"/>
+      <c r="I65" s="82"/>
+      <c r="J65" s="82"/>
+      <c r="K65" s="82"/>
+      <c r="L65" s="82"/>
+      <c r="M65" s="82"/>
+      <c r="N65" s="82"/>
+      <c r="O65" s="82"/>
+      <c r="P65" s="82"/>
+      <c r="Q65" s="82"/>
+      <c r="R65" s="82"/>
+      <c r="S65" s="82"/>
+      <c r="T65" s="82"/>
+      <c r="U65" s="82"/>
+      <c r="V65" s="83"/>
     </row>
     <row r="66" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B66" s="151" t="s">
+      <c r="B66" s="73" t="s">
         <v>141</v>
       </c>
-      <c r="C66" s="152"/>
-      <c r="D66" s="152"/>
-      <c r="E66" s="153"/>
-      <c r="F66" s="157" t="s">
+      <c r="C66" s="74"/>
+      <c r="D66" s="74"/>
+      <c r="E66" s="75"/>
+      <c r="F66" s="79" t="s">
         <v>142</v>
       </c>
-      <c r="G66" s="158"/>
-      <c r="H66" s="158"/>
-      <c r="I66" s="158"/>
-      <c r="J66" s="158"/>
-      <c r="K66" s="158"/>
-      <c r="L66" s="158"/>
-      <c r="M66" s="158"/>
-      <c r="N66" s="158"/>
-      <c r="O66" s="158"/>
-      <c r="P66" s="158"/>
-      <c r="Q66" s="158"/>
-      <c r="R66" s="158"/>
-      <c r="S66" s="158"/>
-      <c r="T66" s="158"/>
-      <c r="U66" s="158"/>
-      <c r="V66" s="159"/>
+      <c r="G66" s="82"/>
+      <c r="H66" s="82"/>
+      <c r="I66" s="82"/>
+      <c r="J66" s="82"/>
+      <c r="K66" s="82"/>
+      <c r="L66" s="82"/>
+      <c r="M66" s="82"/>
+      <c r="N66" s="82"/>
+      <c r="O66" s="82"/>
+      <c r="P66" s="82"/>
+      <c r="Q66" s="82"/>
+      <c r="R66" s="82"/>
+      <c r="S66" s="82"/>
+      <c r="T66" s="82"/>
+      <c r="U66" s="82"/>
+      <c r="V66" s="83"/>
     </row>
     <row r="67" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="154" t="s">
+      <c r="B67" s="90" t="s">
         <v>143</v>
       </c>
-      <c r="C67" s="155"/>
-      <c r="D67" s="155"/>
-      <c r="E67" s="156"/>
-      <c r="F67" s="160" t="s">
+      <c r="C67" s="91"/>
+      <c r="D67" s="91"/>
+      <c r="E67" s="92"/>
+      <c r="F67" s="93" t="s">
         <v>144</v>
       </c>
-      <c r="G67" s="161"/>
-      <c r="H67" s="161"/>
-      <c r="I67" s="161"/>
-      <c r="J67" s="161"/>
-      <c r="K67" s="161"/>
-      <c r="L67" s="161"/>
-      <c r="M67" s="161"/>
-      <c r="N67" s="161"/>
-      <c r="O67" s="161"/>
-      <c r="P67" s="161"/>
-      <c r="Q67" s="161"/>
-      <c r="R67" s="161"/>
-      <c r="S67" s="161"/>
-      <c r="T67" s="161"/>
-      <c r="U67" s="161"/>
-      <c r="V67" s="162"/>
+      <c r="G67" s="94"/>
+      <c r="H67" s="94"/>
+      <c r="I67" s="94"/>
+      <c r="J67" s="94"/>
+      <c r="K67" s="94"/>
+      <c r="L67" s="94"/>
+      <c r="M67" s="94"/>
+      <c r="N67" s="94"/>
+      <c r="O67" s="94"/>
+      <c r="P67" s="94"/>
+      <c r="Q67" s="94"/>
+      <c r="R67" s="94"/>
+      <c r="S67" s="94"/>
+      <c r="T67" s="94"/>
+      <c r="U67" s="94"/>
+      <c r="V67" s="95"/>
     </row>
     <row r="68" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B68" s="34"/>
@@ -4311,6 +4311,68 @@
   </sheetData>
   <sheetProtection password="D20B" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="78">
+    <mergeCell ref="R8:V9"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="R3:V4"/>
+    <mergeCell ref="R6:V6"/>
+    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="C4:K4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="C6:K6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="O8:Q10"/>
+    <mergeCell ref="O24:Q24"/>
+    <mergeCell ref="O12:Q12"/>
+    <mergeCell ref="O13:Q13"/>
+    <mergeCell ref="O14:Q14"/>
+    <mergeCell ref="O15:Q15"/>
+    <mergeCell ref="O16:Q16"/>
+    <mergeCell ref="O17:Q17"/>
+    <mergeCell ref="O18:Q18"/>
+    <mergeCell ref="O19:Q19"/>
+    <mergeCell ref="O20:Q20"/>
+    <mergeCell ref="O23:Q23"/>
+    <mergeCell ref="O21:Q21"/>
+    <mergeCell ref="O22:Q22"/>
+    <mergeCell ref="O25:Q25"/>
+    <mergeCell ref="B26:V26"/>
+    <mergeCell ref="B30:G31"/>
+    <mergeCell ref="I30:O31"/>
+    <mergeCell ref="Q30:R31"/>
+    <mergeCell ref="T30:V31"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="I32:O32"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="T32:V32"/>
+    <mergeCell ref="B35:V35"/>
+    <mergeCell ref="C48:V48"/>
+    <mergeCell ref="B58:E58"/>
+    <mergeCell ref="F57:V57"/>
+    <mergeCell ref="F58:V58"/>
+    <mergeCell ref="F54:V54"/>
+    <mergeCell ref="B37:V37"/>
+    <mergeCell ref="B38:V38"/>
+    <mergeCell ref="C40:V40"/>
+    <mergeCell ref="C41:V41"/>
+    <mergeCell ref="C42:V42"/>
+    <mergeCell ref="C43:V43"/>
+    <mergeCell ref="C52:V52"/>
+    <mergeCell ref="C49:V49"/>
+    <mergeCell ref="C44:V44"/>
+    <mergeCell ref="C45:V45"/>
+    <mergeCell ref="C46:V46"/>
+    <mergeCell ref="C47:V47"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="B66:E66"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="F66:V66"/>
+    <mergeCell ref="F67:V67"/>
+    <mergeCell ref="F64:V64"/>
+    <mergeCell ref="F65:V65"/>
     <mergeCell ref="B63:E63"/>
     <mergeCell ref="D8:D10"/>
     <mergeCell ref="F63:V63"/>
@@ -4327,68 +4389,6 @@
     <mergeCell ref="B61:E61"/>
     <mergeCell ref="B62:E62"/>
     <mergeCell ref="B57:E57"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="B66:E66"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="F66:V66"/>
-    <mergeCell ref="F67:V67"/>
-    <mergeCell ref="F64:V64"/>
-    <mergeCell ref="F65:V65"/>
-    <mergeCell ref="B58:E58"/>
-    <mergeCell ref="F57:V57"/>
-    <mergeCell ref="F58:V58"/>
-    <mergeCell ref="F54:V54"/>
-    <mergeCell ref="B37:V37"/>
-    <mergeCell ref="B38:V38"/>
-    <mergeCell ref="C40:V40"/>
-    <mergeCell ref="C41:V41"/>
-    <mergeCell ref="C42:V42"/>
-    <mergeCell ref="C43:V43"/>
-    <mergeCell ref="C52:V52"/>
-    <mergeCell ref="C49:V49"/>
-    <mergeCell ref="C44:V44"/>
-    <mergeCell ref="C45:V45"/>
-    <mergeCell ref="C46:V46"/>
-    <mergeCell ref="C47:V47"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="I32:O32"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="T32:V32"/>
-    <mergeCell ref="B35:V35"/>
-    <mergeCell ref="C48:V48"/>
-    <mergeCell ref="O25:Q25"/>
-    <mergeCell ref="B26:V26"/>
-    <mergeCell ref="B30:G31"/>
-    <mergeCell ref="I30:O31"/>
-    <mergeCell ref="Q30:R31"/>
-    <mergeCell ref="T30:V31"/>
-    <mergeCell ref="O24:Q24"/>
-    <mergeCell ref="O12:Q12"/>
-    <mergeCell ref="O13:Q13"/>
-    <mergeCell ref="O14:Q14"/>
-    <mergeCell ref="O15:Q15"/>
-    <mergeCell ref="O16:Q16"/>
-    <mergeCell ref="O17:Q17"/>
-    <mergeCell ref="O18:Q18"/>
-    <mergeCell ref="O19:Q19"/>
-    <mergeCell ref="O20:Q20"/>
-    <mergeCell ref="O23:Q23"/>
-    <mergeCell ref="O21:Q21"/>
-    <mergeCell ref="O22:Q22"/>
-    <mergeCell ref="O11:Q11"/>
-    <mergeCell ref="C4:K4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="C6:K6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="O8:Q10"/>
-    <mergeCell ref="R8:V9"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="R3:V4"/>
-    <mergeCell ref="R6:V6"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Limited to 7 Digits" error="Please re-enter as Employee ID is limited to 7 digits long." sqref="N4:O4" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>